<commit_message>
Distance matrix for all samples used in climate analysis (n = 113).
</commit_message>
<xml_diff>
--- a/distance-matrix.xlsx
+++ b/distance-matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="460" windowWidth="19560" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="3280" yWindow="1080" windowWidth="23960" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,350 +29,350 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="113">
   <si>
-    <t>A37114</t>
+    <t>WAM63</t>
   </si>
   <si>
-    <t>A36182</t>
+    <t>WAM60</t>
   </si>
   <si>
-    <t>A35583</t>
+    <t>WAM57</t>
   </si>
   <si>
-    <t>A35582</t>
+    <t>WAM56</t>
   </si>
   <si>
-    <t>A35183</t>
+    <t>WAM55</t>
   </si>
   <si>
-    <t>ABTC114050</t>
+    <t>SAM46</t>
   </si>
   <si>
-    <t>ABTC37891</t>
+    <t>SAM8</t>
   </si>
   <si>
-    <t>ABTC114048</t>
+    <t>SAM44</t>
   </si>
   <si>
-    <t>ABTC143564</t>
+    <t>SAM41</t>
   </si>
   <si>
-    <t>ABTC119685</t>
+    <t>SAM36</t>
   </si>
   <si>
-    <t>A37115</t>
+    <t>WAM64</t>
   </si>
   <si>
-    <t>ABTC113311</t>
+    <t>SAM30</t>
   </si>
   <si>
-    <t>ABTC113310</t>
+    <t>SAM29</t>
   </si>
   <si>
-    <t>ABTC113234</t>
+    <t>SAM28</t>
   </si>
   <si>
-    <t>ABTC113233</t>
+    <t>SAM27</t>
   </si>
   <si>
-    <t>ABTC113232</t>
+    <t>SAM26</t>
   </si>
   <si>
-    <t>ABTC113231</t>
+    <t>SAM25</t>
   </si>
   <si>
-    <t>ABTC85134</t>
+    <t>SAM21</t>
   </si>
   <si>
-    <t>ABTC85133</t>
+    <t>SAM20</t>
   </si>
   <si>
-    <t>ABTC73792</t>
+    <t>SAM18</t>
   </si>
   <si>
-    <t>ABTC73791</t>
+    <t>SAM17</t>
   </si>
   <si>
-    <t>ABTC119496</t>
+    <t>SAM33</t>
   </si>
   <si>
-    <t>ABTC38831</t>
+    <t>SAM16</t>
   </si>
   <si>
-    <t>ABTC38801</t>
+    <t>SAM14</t>
   </si>
   <si>
-    <t>ABTC37976</t>
+    <t>SAM12</t>
   </si>
   <si>
-    <t>ABTC37966</t>
+    <t>SAM11</t>
   </si>
   <si>
-    <t>A35745</t>
+    <t>WAM58</t>
   </si>
   <si>
-    <t>B46574</t>
+    <t>ANWC92</t>
   </si>
   <si>
-    <t>B46525</t>
+    <t>ANWC90</t>
   </si>
   <si>
-    <t>B46415</t>
+    <t>ANWC88</t>
   </si>
   <si>
-    <t>ABTC38802</t>
+    <t>SAM15</t>
   </si>
   <si>
-    <t>B54287</t>
+    <t>ANWC135</t>
   </si>
   <si>
-    <t>B54701</t>
+    <t>ANWC140</t>
   </si>
   <si>
-    <t>B54119</t>
+    <t>ANWC129</t>
   </si>
   <si>
-    <t>B54149</t>
+    <t>ANWC131</t>
   </si>
   <si>
-    <t>B54133</t>
+    <t>ANWC130</t>
   </si>
   <si>
-    <t>B55279</t>
+    <t>ANWC152</t>
   </si>
   <si>
-    <t>ABTC119649</t>
+    <t>SAM35</t>
   </si>
   <si>
-    <t>B55371</t>
+    <t>ANWC159</t>
   </si>
   <si>
-    <t>B52751</t>
+    <t>ANWC118</t>
   </si>
   <si>
-    <t>B53877</t>
+    <t>ANWC119</t>
   </si>
   <si>
-    <t>B41644</t>
+    <t>ANWC84</t>
   </si>
   <si>
-    <t>B46630</t>
+    <t>ANWC94</t>
   </si>
   <si>
-    <t>B54257</t>
+    <t>ANWC133</t>
   </si>
   <si>
-    <t>B54288</t>
+    <t>ANWC136</t>
   </si>
   <si>
-    <t>ABTC113312</t>
+    <t>SAM31</t>
   </si>
   <si>
-    <t>B55292</t>
+    <t>ANWC156</t>
   </si>
   <si>
-    <t>B33180</t>
+    <t>ANWC79</t>
   </si>
   <si>
-    <t>B54256</t>
+    <t>ANWC132</t>
   </si>
   <si>
-    <t>B48315</t>
+    <t>ANWC103</t>
   </si>
   <si>
-    <t>B49330</t>
+    <t>ANWC105</t>
   </si>
   <si>
-    <t>ABTC113313</t>
+    <t>SAM32</t>
   </si>
   <si>
-    <t>B48221</t>
+    <t>ANWC100</t>
   </si>
   <si>
-    <t>ABTC119904</t>
+    <t>SAM39</t>
   </si>
   <si>
-    <t>B48236</t>
+    <t>ANWC102</t>
   </si>
   <si>
-    <t>B54436</t>
+    <t>ANWC138</t>
   </si>
   <si>
-    <t>B48426</t>
+    <t>ANWC104</t>
   </si>
   <si>
-    <t>B55501</t>
+    <t>ANWC168</t>
   </si>
   <si>
-    <t>B52750</t>
+    <t>ANWC117</t>
   </si>
   <si>
-    <t>B48235</t>
+    <t>ANWC101</t>
   </si>
   <si>
-    <t>B29378</t>
+    <t>ANWC69</t>
   </si>
   <si>
-    <t>B32845</t>
+    <t>ANWC75</t>
   </si>
   <si>
-    <t>B55281</t>
+    <t>ANWC154</t>
   </si>
   <si>
-    <t>B49357</t>
+    <t>ANWC106</t>
   </si>
   <si>
-    <t>B49438</t>
+    <t>ANWC108</t>
   </si>
   <si>
-    <t>B50538</t>
+    <t>ANWC112</t>
   </si>
   <si>
-    <t>B49358</t>
+    <t>ANWC107</t>
   </si>
   <si>
-    <t>B54028</t>
+    <t>ANWC126</t>
   </si>
   <si>
-    <t>ABTC114049</t>
+    <t>SAM45</t>
   </si>
   <si>
-    <t>B49626</t>
+    <t>ANWC110</t>
   </si>
   <si>
-    <t>B41656</t>
+    <t>ANWC85</t>
   </si>
   <si>
-    <t>B52745</t>
+    <t>ANWC115</t>
   </si>
   <si>
-    <t>B54435</t>
+    <t>ANWC137</t>
   </si>
   <si>
-    <t>B29336</t>
+    <t>ANWC66</t>
   </si>
   <si>
-    <t>B52746</t>
+    <t>ANWC116</t>
   </si>
   <si>
-    <t>B54458</t>
+    <t>ANWC139</t>
   </si>
   <si>
-    <t>ABTC84315</t>
+    <t>SAM19</t>
   </si>
   <si>
-    <t>B54738</t>
+    <t>ANWC141</t>
   </si>
   <si>
-    <t>B54114</t>
+    <t>ANWC128</t>
   </si>
   <si>
-    <t>B54739</t>
+    <t>ANWC142</t>
   </si>
   <si>
-    <t>B55220</t>
+    <t>ANWC147</t>
   </si>
   <si>
-    <t>B49452</t>
+    <t>ANWC109</t>
   </si>
   <si>
-    <t>B32899</t>
+    <t>ANWC77</t>
   </si>
   <si>
-    <t>B55412</t>
+    <t>ANWC162</t>
   </si>
   <si>
-    <t>B55160</t>
+    <t>ANWC146</t>
   </si>
   <si>
-    <t>ABTC119512</t>
+    <t>SAM34</t>
   </si>
   <si>
-    <t>B55221</t>
+    <t>ANWC148</t>
   </si>
   <si>
-    <t>B55255</t>
+    <t>ANWC150</t>
   </si>
   <si>
-    <t>B55126</t>
+    <t>ANWC145</t>
   </si>
   <si>
-    <t>B55256</t>
+    <t>ANWC151</t>
   </si>
   <si>
-    <t>B52435</t>
+    <t>ANWC113</t>
   </si>
   <si>
-    <t>B55280</t>
+    <t>ANWC153</t>
   </si>
   <si>
-    <t>B55291</t>
+    <t>ANWC155</t>
   </si>
   <si>
-    <t>ABTC119786</t>
+    <t>SAM37</t>
   </si>
   <si>
-    <t>B32011</t>
+    <t>ANWC71</t>
   </si>
   <si>
-    <t>B55308</t>
+    <t>ANWC157</t>
   </si>
   <si>
-    <t>B55370</t>
+    <t>ANWC158</t>
   </si>
   <si>
-    <t>B54740</t>
+    <t>ANWC143</t>
   </si>
   <si>
-    <t>B55399</t>
+    <t>ANWC160</t>
   </si>
   <si>
-    <t>B55400</t>
+    <t>ANWC161</t>
   </si>
   <si>
-    <t>B55503</t>
+    <t>ANWC170</t>
   </si>
   <si>
-    <t>B29377.b</t>
+    <t>ANWC68</t>
   </si>
   <si>
-    <t>B32773</t>
+    <t>ANWC72</t>
   </si>
   <si>
-    <t>B32774</t>
+    <t>ANWC73</t>
   </si>
   <si>
-    <t>B54278</t>
+    <t>ANWC134</t>
   </si>
   <si>
-    <t>B29337.a</t>
+    <t>ANWC67</t>
   </si>
   <si>
-    <t>B33369</t>
+    <t>ANWC81</t>
   </si>
   <si>
-    <t>B55435</t>
+    <t>ANWC163</t>
   </si>
   <si>
-    <t>A36181</t>
+    <t>WAM59</t>
   </si>
   <si>
-    <t>B33013</t>
+    <t>ANWC78</t>
   </si>
   <si>
-    <t>ABTC119851</t>
+    <t>SAM38</t>
   </si>
   <si>
-    <t>B54778</t>
+    <t>ANWC144</t>
   </si>
   <si>
-    <t>B33205</t>
+    <t>ANWC80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,22 +386,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -424,22 +408,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -720,358 +692,354 @@
   <dimension ref="A1:DJ114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BI1" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BJ1" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="5" t="s">
+      <c r="BK1" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BL1" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BM1" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BN1" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BO1" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BP1" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BQ1" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BR1" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BS1" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BT1" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BU1" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="5" t="s">
+      <c r="BV1" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BW1" t="s">
         <v>73</v>
       </c>
-      <c r="BX1" s="5" t="s">
+      <c r="BX1" t="s">
         <v>74</v>
       </c>
-      <c r="BY1" s="5" t="s">
+      <c r="BY1" t="s">
         <v>75</v>
       </c>
-      <c r="BZ1" s="5" t="s">
+      <c r="BZ1" t="s">
         <v>76</v>
       </c>
-      <c r="CA1" s="5" t="s">
+      <c r="CA1" t="s">
         <v>77</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CB1" t="s">
         <v>78</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CC1" t="s">
         <v>79</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CD1" t="s">
         <v>80</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CE1" t="s">
         <v>81</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CF1" t="s">
         <v>82</v>
       </c>
-      <c r="CG1" s="5" t="s">
+      <c r="CG1" t="s">
         <v>83</v>
       </c>
-      <c r="CH1" s="5" t="s">
+      <c r="CH1" t="s">
         <v>84</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CI1" t="s">
         <v>85</v>
       </c>
-      <c r="CJ1" s="5" t="s">
+      <c r="CJ1" t="s">
         <v>86</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CK1" t="s">
         <v>87</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CL1" t="s">
         <v>88</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CM1" t="s">
         <v>89</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CN1" t="s">
         <v>90</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CO1" t="s">
         <v>91</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CP1" t="s">
         <v>92</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CQ1" t="s">
         <v>93</v>
       </c>
-      <c r="CR1" s="5" t="s">
+      <c r="CR1" t="s">
         <v>94</v>
       </c>
-      <c r="CS1" s="5" t="s">
+      <c r="CS1" t="s">
         <v>95</v>
       </c>
-      <c r="CT1" s="5" t="s">
+      <c r="CT1" t="s">
         <v>96</v>
       </c>
-      <c r="CU1" s="5" t="s">
+      <c r="CU1" t="s">
         <v>97</v>
       </c>
-      <c r="CV1" s="5" t="s">
+      <c r="CV1" t="s">
         <v>98</v>
       </c>
-      <c r="CW1" s="5" t="s">
+      <c r="CW1" t="s">
         <v>99</v>
       </c>
-      <c r="CX1" s="5" t="s">
+      <c r="CX1" t="s">
         <v>100</v>
       </c>
-      <c r="CY1" s="5" t="s">
+      <c r="CY1" t="s">
         <v>101</v>
       </c>
-      <c r="CZ1" s="5" t="s">
+      <c r="CZ1" t="s">
         <v>102</v>
       </c>
-      <c r="DA1" s="5" t="s">
+      <c r="DA1" t="s">
         <v>103</v>
       </c>
-      <c r="DB1" s="5" t="s">
+      <c r="DB1" t="s">
         <v>104</v>
       </c>
-      <c r="DC1" s="5" t="s">
+      <c r="DC1" t="s">
         <v>105</v>
       </c>
-      <c r="DD1" s="5" t="s">
+      <c r="DD1" t="s">
         <v>106</v>
       </c>
-      <c r="DE1" s="5" t="s">
+      <c r="DE1" t="s">
         <v>107</v>
       </c>
-      <c r="DF1" s="4" t="s">
+      <c r="DF1" t="s">
         <v>108</v>
       </c>
-      <c r="DG1" s="5" t="s">
+      <c r="DG1" t="s">
         <v>109</v>
       </c>
-      <c r="DH1" s="5" t="s">
+      <c r="DH1" t="s">
         <v>110</v>
       </c>
-      <c r="DI1" s="5" t="s">
+      <c r="DI1" t="s">
         <v>111</v>
       </c>
-      <c r="DJ1" s="5" t="s">
+      <c r="DJ1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -1415,7 +1383,7 @@
       </c>
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1759,7 +1727,7 @@
       </c>
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -2103,7 +2071,7 @@
       </c>
     </row>
     <row r="5" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -2447,7 +2415,7 @@
       </c>
     </row>
     <row r="6" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -2791,7 +2759,7 @@
       </c>
     </row>
     <row r="7" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -3135,7 +3103,7 @@
       </c>
     </row>
     <row r="8" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -3479,7 +3447,7 @@
       </c>
     </row>
     <row r="9" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -3823,7 +3791,7 @@
       </c>
     </row>
     <row r="10" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -4167,7 +4135,7 @@
       </c>
     </row>
     <row r="11" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
@@ -4511,7 +4479,7 @@
       </c>
     </row>
     <row r="12" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -4855,7 +4823,7 @@
       </c>
     </row>
     <row r="13" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1">
@@ -5199,7 +5167,7 @@
       </c>
     </row>
     <row r="14" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1">
@@ -5543,7 +5511,7 @@
       </c>
     </row>
     <row r="15" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1">
@@ -5887,7 +5855,7 @@
       </c>
     </row>
     <row r="16" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1">
@@ -6231,7 +6199,7 @@
       </c>
     </row>
     <row r="17" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1">
@@ -6575,7 +6543,7 @@
       </c>
     </row>
     <row r="18" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1">
@@ -6919,7 +6887,7 @@
       </c>
     </row>
     <row r="19" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1">
@@ -7263,7 +7231,7 @@
       </c>
     </row>
     <row r="20" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1">
@@ -7607,7 +7575,7 @@
       </c>
     </row>
     <row r="21" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1">
@@ -7951,7 +7919,7 @@
       </c>
     </row>
     <row r="22" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1">
@@ -8295,7 +8263,7 @@
       </c>
     </row>
     <row r="23" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1">
@@ -8639,7 +8607,7 @@
       </c>
     </row>
     <row r="24" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="1">
@@ -8983,7 +8951,7 @@
       </c>
     </row>
     <row r="25" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1">
@@ -9327,7 +9295,7 @@
       </c>
     </row>
     <row r="26" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="1">
@@ -9671,7 +9639,7 @@
       </c>
     </row>
     <row r="27" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="1">
@@ -10015,7 +9983,7 @@
       </c>
     </row>
     <row r="28" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="1">
@@ -10359,7 +10327,7 @@
       </c>
     </row>
     <row r="29" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="1">
@@ -10703,7 +10671,7 @@
       </c>
     </row>
     <row r="30" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="1">
@@ -11047,7 +11015,7 @@
       </c>
     </row>
     <row r="31" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="1">
@@ -11391,7 +11359,7 @@
       </c>
     </row>
     <row r="32" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="1">
@@ -11735,7 +11703,7 @@
       </c>
     </row>
     <row r="33" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="1">
@@ -12079,7 +12047,7 @@
       </c>
     </row>
     <row r="34" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="1">
@@ -12423,7 +12391,7 @@
       </c>
     </row>
     <row r="35" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="1">
@@ -12767,7 +12735,7 @@
       </c>
     </row>
     <row r="36" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="1">
@@ -13111,7 +13079,7 @@
       </c>
     </row>
     <row r="37" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" s="1">
@@ -13455,7 +13423,7 @@
       </c>
     </row>
     <row r="38" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="1">
@@ -13799,7 +13767,7 @@
       </c>
     </row>
     <row r="39" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="1">
@@ -14143,7 +14111,7 @@
       </c>
     </row>
     <row r="40" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="1">
@@ -14487,7 +14455,7 @@
       </c>
     </row>
     <row r="41" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="1">
@@ -14831,7 +14799,7 @@
       </c>
     </row>
     <row r="42" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="1">
@@ -15175,7 +15143,7 @@
       </c>
     </row>
     <row r="43" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="1">
@@ -15519,7 +15487,7 @@
       </c>
     </row>
     <row r="44" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
+      <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="1">
@@ -15863,7 +15831,7 @@
       </c>
     </row>
     <row r="45" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="1">
@@ -16207,7 +16175,7 @@
       </c>
     </row>
     <row r="46" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="1">
@@ -16551,7 +16519,7 @@
       </c>
     </row>
     <row r="47" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="1">
@@ -16895,7 +16863,7 @@
       </c>
     </row>
     <row r="48" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="1">
@@ -17239,7 +17207,7 @@
       </c>
     </row>
     <row r="49" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49" s="1">
@@ -17583,7 +17551,7 @@
       </c>
     </row>
     <row r="50" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A50" s="5" t="s">
+      <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50" s="1">
@@ -17927,7 +17895,7 @@
       </c>
     </row>
     <row r="51" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="1">
@@ -18271,7 +18239,7 @@
       </c>
     </row>
     <row r="52" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="1">
@@ -18615,7 +18583,7 @@
       </c>
     </row>
     <row r="53" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="1">
@@ -18959,7 +18927,7 @@
       </c>
     </row>
     <row r="54" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="1">
@@ -19303,7 +19271,7 @@
       </c>
     </row>
     <row r="55" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="1">
@@ -19647,7 +19615,7 @@
       </c>
     </row>
     <row r="56" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="1">
@@ -19991,7 +19959,7 @@
       </c>
     </row>
     <row r="57" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A57" s="5" t="s">
+      <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="1">
@@ -20335,7 +20303,7 @@
       </c>
     </row>
     <row r="58" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A58" s="5" t="s">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58" s="1">
@@ -20679,7 +20647,7 @@
       </c>
     </row>
     <row r="59" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A59" s="5" t="s">
+      <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="1">
@@ -21023,7 +20991,7 @@
       </c>
     </row>
     <row r="60" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A60" s="5" t="s">
+      <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="1">
@@ -21367,7 +21335,7 @@
       </c>
     </row>
     <row r="61" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A61" s="5" t="s">
+      <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61" s="1">
@@ -21711,7 +21679,7 @@
       </c>
     </row>
     <row r="62" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A62" s="5" t="s">
+      <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62" s="1">
@@ -22055,7 +22023,7 @@
       </c>
     </row>
     <row r="63" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63" s="1">
@@ -22399,7 +22367,7 @@
       </c>
     </row>
     <row r="64" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A64" s="5" t="s">
+      <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64" s="1">
@@ -22743,7 +22711,7 @@
       </c>
     </row>
     <row r="65" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A65" s="5" t="s">
+      <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65" s="1">
@@ -23087,7 +23055,7 @@
       </c>
     </row>
     <row r="66" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
+      <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66" s="1">
@@ -23431,7 +23399,7 @@
       </c>
     </row>
     <row r="67" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
+      <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="1">
@@ -23775,7 +23743,7 @@
       </c>
     </row>
     <row r="68" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
+      <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="1">
@@ -24119,7 +24087,7 @@
       </c>
     </row>
     <row r="69" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A69" s="5" t="s">
+      <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69" s="1">
@@ -24463,7 +24431,7 @@
       </c>
     </row>
     <row r="70" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
+      <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70" s="1">
@@ -24807,7 +24775,7 @@
       </c>
     </row>
     <row r="71" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A71" s="5" t="s">
+      <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71" s="1">
@@ -25151,7 +25119,7 @@
       </c>
     </row>
     <row r="72" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A72" s="5" t="s">
+      <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72" s="1">
@@ -25495,7 +25463,7 @@
       </c>
     </row>
     <row r="73" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A73" s="5" t="s">
+      <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="1">
@@ -25839,7 +25807,7 @@
       </c>
     </row>
     <row r="74" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A74" s="5" t="s">
+      <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="1">
@@ -26183,7 +26151,7 @@
       </c>
     </row>
     <row r="75" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A75" s="5" t="s">
+      <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="B75" s="1">
@@ -26527,7 +26495,7 @@
       </c>
     </row>
     <row r="76" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A76" s="5" t="s">
+      <c r="A76" t="s">
         <v>74</v>
       </c>
       <c r="B76" s="1">
@@ -26871,7 +26839,7 @@
       </c>
     </row>
     <row r="77" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
+      <c r="A77" t="s">
         <v>75</v>
       </c>
       <c r="B77" s="1">
@@ -27215,7 +27183,7 @@
       </c>
     </row>
     <row r="78" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+      <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="B78" s="1">
@@ -27559,7 +27527,7 @@
       </c>
     </row>
     <row r="79" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+      <c r="A79" t="s">
         <v>77</v>
       </c>
       <c r="B79" s="1">
@@ -27903,7 +27871,7 @@
       </c>
     </row>
     <row r="80" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A80" s="5" t="s">
+      <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="B80" s="1">
@@ -28247,7 +28215,7 @@
       </c>
     </row>
     <row r="81" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A81" s="5" t="s">
+      <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81" s="1">
@@ -28591,7 +28559,7 @@
       </c>
     </row>
     <row r="82" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A82" s="5" t="s">
+      <c r="A82" t="s">
         <v>80</v>
       </c>
       <c r="B82" s="1">
@@ -28935,7 +28903,7 @@
       </c>
     </row>
     <row r="83" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A83" s="5" t="s">
+      <c r="A83" t="s">
         <v>81</v>
       </c>
       <c r="B83" s="1">
@@ -29279,7 +29247,7 @@
       </c>
     </row>
     <row r="84" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A84" s="5" t="s">
+      <c r="A84" t="s">
         <v>82</v>
       </c>
       <c r="B84" s="1">
@@ -29623,7 +29591,7 @@
       </c>
     </row>
     <row r="85" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" t="s">
         <v>83</v>
       </c>
       <c r="B85" s="1">
@@ -29967,7 +29935,7 @@
       </c>
     </row>
     <row r="86" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A86" s="5" t="s">
+      <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="B86" s="1">
@@ -30311,7 +30279,7 @@
       </c>
     </row>
     <row r="87" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A87" s="5" t="s">
+      <c r="A87" t="s">
         <v>85</v>
       </c>
       <c r="B87" s="1">
@@ -30655,7 +30623,7 @@
       </c>
     </row>
     <row r="88" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A88" s="5" t="s">
+      <c r="A88" t="s">
         <v>86</v>
       </c>
       <c r="B88" s="1">
@@ -30999,7 +30967,7 @@
       </c>
     </row>
     <row r="89" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A89" s="5" t="s">
+      <c r="A89" t="s">
         <v>87</v>
       </c>
       <c r="B89" s="1">
@@ -31343,7 +31311,7 @@
       </c>
     </row>
     <row r="90" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A90" s="5" t="s">
+      <c r="A90" t="s">
         <v>88</v>
       </c>
       <c r="B90" s="1">
@@ -31687,7 +31655,7 @@
       </c>
     </row>
     <row r="91" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A91" s="5" t="s">
+      <c r="A91" t="s">
         <v>89</v>
       </c>
       <c r="B91" s="1">
@@ -32031,7 +31999,7 @@
       </c>
     </row>
     <row r="92" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A92" s="5" t="s">
+      <c r="A92" t="s">
         <v>90</v>
       </c>
       <c r="B92" s="1">
@@ -32375,7 +32343,7 @@
       </c>
     </row>
     <row r="93" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A93" s="5" t="s">
+      <c r="A93" t="s">
         <v>91</v>
       </c>
       <c r="B93" s="1">
@@ -32719,7 +32687,7 @@
       </c>
     </row>
     <row r="94" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A94" s="5" t="s">
+      <c r="A94" t="s">
         <v>92</v>
       </c>
       <c r="B94" s="1">
@@ -33063,7 +33031,7 @@
       </c>
     </row>
     <row r="95" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A95" s="5" t="s">
+      <c r="A95" t="s">
         <v>93</v>
       </c>
       <c r="B95" s="1">
@@ -33407,7 +33375,7 @@
       </c>
     </row>
     <row r="96" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
+      <c r="A96" t="s">
         <v>94</v>
       </c>
       <c r="B96" s="1">
@@ -33751,7 +33719,7 @@
       </c>
     </row>
     <row r="97" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
+      <c r="A97" t="s">
         <v>95</v>
       </c>
       <c r="B97" s="1">
@@ -34095,7 +34063,7 @@
       </c>
     </row>
     <row r="98" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
+      <c r="A98" t="s">
         <v>96</v>
       </c>
       <c r="B98" s="1">
@@ -34439,7 +34407,7 @@
       </c>
     </row>
     <row r="99" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
+      <c r="A99" t="s">
         <v>97</v>
       </c>
       <c r="B99" s="1">
@@ -34783,7 +34751,7 @@
       </c>
     </row>
     <row r="100" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A100" s="5" t="s">
+      <c r="A100" t="s">
         <v>98</v>
       </c>
       <c r="B100" s="1">
@@ -35127,7 +35095,7 @@
       </c>
     </row>
     <row r="101" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A101" s="5" t="s">
+      <c r="A101" t="s">
         <v>99</v>
       </c>
       <c r="B101" s="1">
@@ -35471,7 +35439,7 @@
       </c>
     </row>
     <row r="102" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A102" s="5" t="s">
+      <c r="A102" t="s">
         <v>100</v>
       </c>
       <c r="B102" s="1">
@@ -35815,7 +35783,7 @@
       </c>
     </row>
     <row r="103" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A103" s="5" t="s">
+      <c r="A103" t="s">
         <v>101</v>
       </c>
       <c r="B103" s="1">
@@ -36159,7 +36127,7 @@
       </c>
     </row>
     <row r="104" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A104" s="5" t="s">
+      <c r="A104" t="s">
         <v>102</v>
       </c>
       <c r="B104" s="1">
@@ -36503,7 +36471,7 @@
       </c>
     </row>
     <row r="105" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A105" s="5" t="s">
+      <c r="A105" t="s">
         <v>103</v>
       </c>
       <c r="B105" s="1">
@@ -36847,7 +36815,7 @@
       </c>
     </row>
     <row r="106" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A106" s="5" t="s">
+      <c r="A106" t="s">
         <v>104</v>
       </c>
       <c r="B106" s="1">
@@ -37191,7 +37159,7 @@
       </c>
     </row>
     <row r="107" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A107" s="5" t="s">
+      <c r="A107" t="s">
         <v>105</v>
       </c>
       <c r="B107" s="1">
@@ -37535,7 +37503,7 @@
       </c>
     </row>
     <row r="108" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
+      <c r="A108" t="s">
         <v>106</v>
       </c>
       <c r="B108" s="1">
@@ -37879,7 +37847,7 @@
       </c>
     </row>
     <row r="109" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
+      <c r="A109" t="s">
         <v>107</v>
       </c>
       <c r="B109" s="1">
@@ -38223,7 +38191,7 @@
       </c>
     </row>
     <row r="110" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
+      <c r="A110" t="s">
         <v>108</v>
       </c>
       <c r="B110" s="1">
@@ -38567,7 +38535,7 @@
       </c>
     </row>
     <row r="111" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
+      <c r="A111" t="s">
         <v>109</v>
       </c>
       <c r="B111" s="1">
@@ -38911,7 +38879,7 @@
       </c>
     </row>
     <row r="112" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
+      <c r="A112" t="s">
         <v>110</v>
       </c>
       <c r="B112" s="1">
@@ -39255,7 +39223,7 @@
       </c>
     </row>
     <row r="113" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
+      <c r="A113" t="s">
         <v>111</v>
       </c>
       <c r="B113" s="1">
@@ -39599,7 +39567,7 @@
       </c>
     </row>
     <row r="114" spans="1:114" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
+      <c r="A114" t="s">
         <v>112</v>
       </c>
       <c r="B114" s="1">

</xml_diff>